<commit_message>
added indicators plus document
</commit_message>
<xml_diff>
--- a/Main/MWD sources Fig 03_source.xlsx
+++ b/Main/MWD sources Fig 03_source.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armen\Desktop\Drought Impacts\SoCal Indicators\Main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armen\Desktop\Drought Indicators - SoCal\Main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC78D34-1FCA-4ACE-8A03-D82479EC2CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EAD548-D5B9-4890-A06C-40768021331E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MWDHistoricSupply" sheetId="6" r:id="rId1"/>
@@ -11626,84 +11626,84 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Aqueduct!$F$17:$F$41</c:f>
+              <c:f>Aqueduct!$G$17:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.25277777777777699</c:v>
+                  <c:v>0.23703703703703699</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.227777777777777</c:v>
+                  <c:v>0.194444444444444</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58055555555555505</c:v>
+                  <c:v>0.61388888888888804</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31944444444444398</c:v>
+                  <c:v>0.219444444444444</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.84722222222222199</c:v>
+                  <c:v>0.87222222222222201</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73611111111111105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.77500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.655555555555555</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.68333333333333302</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.83055555555555505</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.51666666666666605</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.49444444444444402</c:v>
+                  <c:v>0.43055555555555503</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.55555555555555503</c:v>
+                  <c:v>0.52500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48611111111111099</c:v>
+                  <c:v>0.47222222222222199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.57222222222222197</c:v>
+                  <c:v>0.61388888888888804</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.54722222222222205</c:v>
+                  <c:v>0.452777777777777</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>0.87777777777777699</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.85277777777777697</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.358333333333333</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.35277777777777702</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.46111111111111103</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.66111111111111098</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>0.83333333333333304</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.82222222222222197</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.241666666666666</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.38333333333333303</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.563888888888888</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.67500000000000004</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.83888888888888802</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.344444444444444</c:v>
+                  <c:v>0.42777777777777698</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22222222222222199</c:v>
+                  <c:v>0.28333333333333299</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.6111111111110999E-2</c:v>
+                  <c:v>0.11944444444444401</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.105555555555555</c:v>
+                  <c:v>6.1111111111110998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11916,36 +11916,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -12240,6 +12210,141 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DF70-4526-AA76-F13818D28A77}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Aqueduct!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Imports Portfolio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Aqueduct!$B$28:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Aqueduct!$E$28:$E$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>218400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>207300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>202600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>339799.99999999901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>365800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>185799.99999999898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>241600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>324900</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>74500</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>51500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-952A-4D39-B57D-05974ED814FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12275,6 +12380,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -12337,6 +12497,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Supply af)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -12386,6 +12601,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -23819,7 +24065,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24506,7 +24752,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="12992100" cy="9436100"/>
+    <xdr:ext cx="8665221" cy="6288186"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -25077,14 +25323,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B41"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -27665,14 +27911,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE63D60-F20A-4BE8-A537-84C8DA5529FC}">
   <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="28.5" customHeight="1">
@@ -28012,7 +28258,7 @@
         <v>0.61388888888888804</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" ref="H29:H50" si="1">C29-E29</f>
+        <f t="shared" ref="H29:H41" si="1">C29-E29</f>
         <v>44700</v>
       </c>
     </row>
@@ -28435,15 +28681,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{773C619C-38B7-441A-B4DE-3FCE17381564}">
   <dimension ref="B1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
@@ -29219,11 +29465,11 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6328125" customWidth="1"/>
-    <col min="28" max="28" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="28" max="28" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:46">
@@ -29264,7 +29510,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="19">
+    <row r="2" spans="1:46" ht="18.75">
       <c r="A2">
         <v>1976</v>
       </c>
@@ -29369,7 +29615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="19">
+    <row r="3" spans="1:46" ht="18.75">
       <c r="A3">
         <v>1977</v>
       </c>
@@ -29474,7 +29720,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="19">
+    <row r="4" spans="1:46" ht="18.75">
       <c r="A4">
         <v>1978</v>
       </c>
@@ -29580,7 +29826,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="19">
+    <row r="5" spans="1:46" ht="18.75">
       <c r="A5">
         <v>1979</v>
       </c>
@@ -29686,7 +29932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="19">
+    <row r="6" spans="1:46" ht="18.75">
       <c r="A6">
         <v>1980</v>
       </c>
@@ -29792,7 +30038,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="19">
+    <row r="7" spans="1:46" ht="18.75">
       <c r="A7">
         <v>1981</v>
       </c>
@@ -29898,7 +30144,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:46" ht="19">
+    <row r="8" spans="1:46" ht="18.75">
       <c r="A8">
         <v>1982</v>
       </c>
@@ -30004,7 +30250,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="19">
+    <row r="9" spans="1:46" ht="18.75">
       <c r="A9">
         <v>1983</v>
       </c>
@@ -30110,7 +30356,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="19">
+    <row r="10" spans="1:46" ht="18.75">
       <c r="A10">
         <v>1984</v>
       </c>
@@ -30216,7 +30462,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="19">
+    <row r="11" spans="1:46" ht="18.75">
       <c r="A11">
         <v>1985</v>
       </c>
@@ -30322,7 +30568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:46" ht="19">
+    <row r="12" spans="1:46" ht="18.75">
       <c r="A12">
         <v>1986</v>
       </c>
@@ -30428,7 +30674,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:46" ht="19">
+    <row r="13" spans="1:46" ht="18.75">
       <c r="A13">
         <v>1987</v>
       </c>
@@ -30534,7 +30780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:46" ht="19">
+    <row r="14" spans="1:46" ht="18.75">
       <c r="A14">
         <v>1988</v>
       </c>
@@ -30639,7 +30885,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:46" ht="19">
+    <row r="15" spans="1:46" ht="18.75">
       <c r="A15">
         <v>1989</v>
       </c>
@@ -30745,7 +30991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:46" ht="19">
+    <row r="16" spans="1:46" ht="18.75">
       <c r="A16">
         <v>1990</v>
       </c>
@@ -30851,7 +31097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:46" ht="19">
+    <row r="17" spans="1:46" ht="18.75">
       <c r="A17">
         <v>1991</v>
       </c>
@@ -30957,7 +31203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:46" ht="19">
+    <row r="18" spans="1:46" ht="18.75">
       <c r="A18">
         <v>1992</v>
       </c>
@@ -31063,7 +31309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:46" ht="19">
+    <row r="19" spans="1:46" ht="18.75">
       <c r="A19">
         <v>1993</v>
       </c>
@@ -31169,7 +31415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:46" ht="19">
+    <row r="20" spans="1:46" ht="18.75">
       <c r="A20">
         <v>1994</v>
       </c>
@@ -31274,7 +31520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:46" ht="19">
+    <row r="21" spans="1:46" ht="18.75">
       <c r="A21">
         <v>1995</v>
       </c>
@@ -31380,7 +31626,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:46" ht="19">
+    <row r="22" spans="1:46" ht="18.75">
       <c r="A22">
         <v>1996</v>
       </c>
@@ -31486,7 +31732,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:46" ht="19">
+    <row r="23" spans="1:46" ht="18.75">
       <c r="A23">
         <v>1997</v>
       </c>
@@ -31592,7 +31838,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:46" ht="19">
+    <row r="24" spans="1:46" ht="18.75">
       <c r="A24">
         <v>1998</v>
       </c>
@@ -31698,7 +31944,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:46" ht="19">
+    <row r="25" spans="1:46" ht="18.75">
       <c r="A25">
         <v>1999</v>
       </c>
@@ -31804,7 +32050,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:46" ht="19">
+    <row r="26" spans="1:46" ht="18.75">
       <c r="A26">
         <v>2000</v>
       </c>
@@ -31910,7 +32156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:46" ht="19">
+    <row r="27" spans="1:46" ht="18.75">
       <c r="A27">
         <v>2001</v>
       </c>
@@ -32016,7 +32262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:46" ht="19">
+    <row r="28" spans="1:46" ht="18.75">
       <c r="A28">
         <v>2002</v>
       </c>
@@ -32122,7 +32368,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:46" ht="19">
+    <row r="29" spans="1:46" ht="18.75">
       <c r="A29">
         <v>2003</v>
       </c>
@@ -32228,7 +32474,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:46" ht="19">
+    <row r="30" spans="1:46" ht="18.75">
       <c r="A30">
         <v>2004</v>
       </c>
@@ -32334,7 +32580,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:46" ht="19">
+    <row r="31" spans="1:46" ht="18.75">
       <c r="A31">
         <v>2005</v>
       </c>
@@ -32440,7 +32686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:46" ht="19">
+    <row r="32" spans="1:46" ht="18.75">
       <c r="A32">
         <v>2006</v>
       </c>
@@ -32546,7 +32792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:46" ht="19">
+    <row r="33" spans="1:46" ht="18.75">
       <c r="A33">
         <v>2007</v>
       </c>
@@ -32652,7 +32898,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:46" ht="19">
+    <row r="34" spans="1:46" ht="18.75">
       <c r="A34">
         <v>2008</v>
       </c>
@@ -32758,7 +33004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:46" ht="19">
+    <row r="35" spans="1:46" ht="18.75">
       <c r="A35">
         <v>2009</v>
       </c>
@@ -32863,7 +33109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:46" ht="19">
+    <row r="36" spans="1:46" ht="18.75">
       <c r="A36">
         <v>2010</v>
       </c>
@@ -32969,7 +33215,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:46" ht="19">
+    <row r="37" spans="1:46" ht="18.75">
       <c r="A37">
         <v>2011</v>
       </c>
@@ -33075,7 +33321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:46" ht="19">
+    <row r="38" spans="1:46" ht="18.75">
       <c r="A38">
         <v>2012</v>
       </c>
@@ -33181,7 +33427,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:46" ht="19">
+    <row r="39" spans="1:46" ht="18.75">
       <c r="A39">
         <v>2013</v>
       </c>
@@ -33287,7 +33533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:46" ht="19">
+    <row r="40" spans="1:46" ht="18.75">
       <c r="A40">
         <v>2014</v>
       </c>
@@ -33393,7 +33639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:46" ht="19">
+    <row r="41" spans="1:46" ht="18.75">
       <c r="A41">
         <v>2015</v>
       </c>
@@ -33499,7 +33745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:46" ht="19">
+    <row r="42" spans="1:46" ht="18.75">
       <c r="W42">
         <v>1934</v>
       </c>
@@ -33544,7 +33790,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:46" ht="19">
+    <row r="43" spans="1:46" ht="18.75">
       <c r="W43">
         <v>1935</v>
       </c>
@@ -33589,7 +33835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:46" ht="19">
+    <row r="44" spans="1:46" ht="18.75">
       <c r="W44">
         <v>1936</v>
       </c>
@@ -33634,7 +33880,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:46" ht="19">
+    <row r="45" spans="1:46" ht="18.75">
       <c r="W45">
         <v>1937</v>
       </c>
@@ -33679,7 +33925,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:46" ht="19">
+    <row r="46" spans="1:46" ht="18.75">
       <c r="W46">
         <v>1938</v>
       </c>
@@ -33724,7 +33970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:46" ht="19">
+    <row r="47" spans="1:46" ht="18.75">
       <c r="W47">
         <v>1939</v>
       </c>
@@ -33769,7 +34015,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:46" ht="19">
+    <row r="48" spans="1:46" ht="18.75">
       <c r="W48">
         <v>1940</v>
       </c>

</xml_diff>